<commit_message>
Datamodel, UC1-OC, glossary (antal personer) updated
</commit_message>
<xml_diff>
--- a/UPDokument/Glossary.xlsx
+++ b/UPDokument/Glossary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juyoung Choi\iCloudDrive\eclipse\flextur\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juyoung Choi\iCloudDrive\eclipse\flextur\UPDokument\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
   <si>
     <t>Glossary</t>
   </si>
@@ -262,6 +262,30 @@
   </si>
   <si>
     <t>13-16 tilføjet</t>
+  </si>
+  <si>
+    <t>antalPersoner</t>
+  </si>
+  <si>
+    <t>antal af personer der bestiller den tur</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>antal passegerer : same but change to antalPersoner</t>
+  </si>
+  <si>
+    <t>Elaboration draft1</t>
+  </si>
+  <si>
+    <t>13.maj 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 : antal personer </t>
+  </si>
+  <si>
+    <t>Jonas og Juyoung Choi</t>
   </si>
 </sst>
 </file>
@@ -704,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,7 +739,7 @@
     <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" customWidth="1"/>
     <col min="3" max="3" width="65" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -858,6 +882,20 @@
       </c>
       <c r="D13" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -878,7 +916,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1180,16 +1218,24 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>17</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="B20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="8">

</xml_diff>

<commit_message>
UC7,8 formelle usecase done
</commit_message>
<xml_diff>
--- a/UPDokument/Glossary.xlsx
+++ b/UPDokument/Glossary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15840" windowHeight="5772" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15840" windowHeight="5772"/>
   </bookViews>
   <sheets>
     <sheet name="Revision list" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="115">
   <si>
     <t>Glossary</t>
   </si>
@@ -225,9 +225,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>MidtTrafik virksomhed, Chef af MidtTrafik</t>
-  </si>
-  <si>
     <t>Inception draft 8</t>
   </si>
   <si>
@@ -325,6 +322,54 @@
   </si>
   <si>
     <t>okhttp-2.5.0.jar, okio</t>
+  </si>
+  <si>
+    <t>MidtTrafik virksomhed</t>
+  </si>
+  <si>
+    <t>interessenter</t>
+  </si>
+  <si>
+    <t>midtTrafiks chef</t>
+  </si>
+  <si>
+    <t>MidtTrafiks direktør</t>
+  </si>
+  <si>
+    <t>personllige oplysninger af kunde</t>
+  </si>
+  <si>
+    <t>profil oplysninger, kunde oplysninger, kundeoplysninger</t>
+  </si>
+  <si>
+    <t>Elaboration draft4</t>
+  </si>
+  <si>
+    <t>24. maj 2016</t>
+  </si>
+  <si>
+    <t>opret bruger</t>
+  </si>
+  <si>
+    <t>opret kunde, opret en ny kunde</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>brugergræsnflade for FlexturSystem</t>
+  </si>
+  <si>
+    <t>gui, skærme</t>
+  </si>
+  <si>
+    <t>UC7</t>
+  </si>
+  <si>
+    <t>opret  en kundeprofil i GUI :</t>
+  </si>
+  <si>
+    <t>20, 21 opret profil : kundeoplysninger = profiloplysninger, 22 : opret bruger = kunde</t>
   </si>
 </sst>
 </file>
@@ -392,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -433,11 +478,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -479,12 +530,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:D16" totalsRowShown="0">
-  <autoFilter ref="A5:D16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:D17" totalsRowShown="0">
+  <autoFilter ref="A5:D17"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Version"/>
     <tableColumn id="2" name="Date"/>
-    <tableColumn id="3" name="Description"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
     <tableColumn id="4" name="Author"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -492,16 +543,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:G44" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:G44" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A3:G44"/>
   <tableColumns count="7">
-    <tableColumn id="7" name="ID" dataDxfId="6"/>
-    <tableColumn id="1" name="Term" dataDxfId="5"/>
-    <tableColumn id="2" name="Definition and information" dataDxfId="4"/>
-    <tableColumn id="6" name="Specifik UC reference" dataDxfId="3"/>
-    <tableColumn id="3" name="Format" dataDxfId="2"/>
-    <tableColumn id="4" name="Validation Rules" dataDxfId="1"/>
-    <tableColumn id="5" name="Aliases" dataDxfId="0"/>
+    <tableColumn id="7" name="ID" dataDxfId="7"/>
+    <tableColumn id="1" name="Term" dataDxfId="6"/>
+    <tableColumn id="2" name="Definition and information" dataDxfId="5"/>
+    <tableColumn id="6" name="Specifik UC reference" dataDxfId="4"/>
+    <tableColumn id="3" name="Format" dataDxfId="3"/>
+    <tableColumn id="4" name="Validation Rules" dataDxfId="2"/>
+    <tableColumn id="5" name="Aliases" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -770,17 +821,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -789,7 +840,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="11"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -797,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="11"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -807,7 +858,7 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
@@ -821,7 +872,7 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
@@ -835,7 +886,7 @@
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D7" t="s">
@@ -849,7 +900,7 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D8" t="s">
@@ -863,7 +914,7 @@
       <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D9" t="s">
@@ -877,7 +928,7 @@
       <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D10" t="s">
@@ -891,7 +942,7 @@
       <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D11" t="s">
@@ -903,10 +954,10 @@
         <v>63</v>
       </c>
       <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C12" t="s">
-        <v>69</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -914,13 +965,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" t="s">
-        <v>78</v>
+      <c r="C13" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -928,27 +979,27 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
         <v>83</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>85</v>
-      </c>
-      <c r="D14" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
         <v>87</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>89</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -956,23 +1007,33 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>96</v>
       </c>
-      <c r="D16" t="s">
-        <v>97</v>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -985,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1033,7 +1094,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1046,7 +1107,7 @@
       <c r="D4" s="1"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1230,7 +1291,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1238,7 +1299,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>61</v>
@@ -1249,7 +1310,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1257,10 +1318,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>60</v>
@@ -1276,16 +1337,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
@@ -1293,18 +1354,18 @@
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -1312,13 +1373,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -1329,63 +1390,89 @@
         <v>19</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>20</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="1"/>
+      <c r="B23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G23" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>21</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="1"/>
+      <c r="B24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G24" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>22</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="B25" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>23</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="1"/>
+      <c r="B26" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="8">

</xml_diff>